<commit_message>
Day Calendar test done
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/CrmAppTestData.xlsx
+++ b/src/test/resources/TestData/CrmAppTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamkhan/IdeaProjects/CRMPOM/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AC1672-489D-E74E-86C6-D810A8468808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A92E58B-464D-DE46-B2BF-391854BAD4EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860" activeTab="1" xr2:uid="{835F5C3E-8192-E742-8AD3-2168444FCE94}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860" activeTab="2" xr2:uid="{835F5C3E-8192-E742-8AD3-2168444FCE94}"/>
   </bookViews>
   <sheets>
     <sheet name="LeftSideBar" sheetId="1" r:id="rId1"/>
@@ -848,7 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107F4C93-B820-3D46-B6F8-6EABC5430A8F}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2A4F4C-C45A-7C44-B8AB-F5E7331E5277}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Started On sorting of ColumnHEader functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/CrmAppTestData.xlsx
+++ b/src/test/resources/TestData/CrmAppTestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamkhan/IdeaProjects/CRMPOM/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A92E58B-464D-DE46-B2BF-391854BAD4EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DFB39D-1820-1141-9C52-51E065B5E152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860" activeTab="2" xr2:uid="{835F5C3E-8192-E742-8AD3-2168444FCE94}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860" activeTab="3" xr2:uid="{835F5C3E-8192-E742-8AD3-2168444FCE94}"/>
   </bookViews>
   <sheets>
     <sheet name="LeftSideBar" sheetId="1" r:id="rId1"/>
     <sheet name="SideBarUrls" sheetId="2" r:id="rId2"/>
     <sheet name="NewEvent" sheetId="3" r:id="rId3"/>
+    <sheet name="verifyContactHeaders" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="118">
   <si>
     <t>Home</t>
   </si>
@@ -371,6 +372,24 @@
   </si>
   <si>
     <t>Company8</t>
+  </si>
+  <si>
+    <t>ContactHeader</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Options</t>
   </si>
 </sst>
 </file>
@@ -441,13 +460,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -985,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2A4F4C-C45A-7C44-B8AB-F5E7331E5277}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -1348,4 +1368,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF3C7265-4592-A643-B4C7-1F24CC5A9386}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>